<commit_message>
Add heating support, custom generators, and UI improvements
Major update to app adding support for:
- added ability to handle heating tents in cold weather environments
- custom generator file uploads
- E2O logo display in app
- improved UI dialogs.

The MILP formulation and ECU input files were updated to support new data for heating and cooling.
Requirements updated to include gitpython for update date display.
Various bug fixes, refactoring, and enhancements to plotting, data validation, and user feedback.
</commit_message>
<xml_diff>
--- a/Inputs/ECUSpecs.xlsx
+++ b/Inputs/ECUSpecs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmc-my.sharepoint-mil.us/personal/deryk_l_clary_mil_usmc_mil/Documents/Documents/VS Code/1. Air Conditioners/Inputs/XLS Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmc-my.sharepoint-mil.us/personal/deryk_l_clary_mil_usmc_mil/Documents/Documents/VS Code/1. Air Conditioners/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{119B4761-BC1C-411D-80A4-A6DC2720C6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2586C56C-4A96-49B5-9E04-EAD45C933CBC}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{119B4761-BC1C-411D-80A4-A6DC2720C6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19562F0D-D24C-4BE5-B6F1-537A969544A0}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="90" windowWidth="29040" windowHeight="15510" xr2:uid="{60A86E40-7E2F-4C45-AF44-FF6C3ADE04BA}"/>
+    <workbookView xWindow="30045" yWindow="1845" windowWidth="21600" windowHeight="11070" xr2:uid="{60A86E40-7E2F-4C45-AF44-FF6C3ADE04BA}"/>
   </bookViews>
   <sheets>
     <sheet name="ECUSpecs" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-The maximum BTU/hr capacity</t>
+The maximum BTU/hr capacity
+Using "@ 125 degrees" metrics.</t>
         </r>
       </text>
     </comment>
@@ -131,11 +132,36 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-The maximum amount of electrical load produced by the unit.</t>
+The maximum amount of electrical load produced by the unit.
+Using "@ 125 degrees" metrics.</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{CA22DA69-A337-4697-92E5-7140B25277EF}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{7753F88A-6B92-4534-9A04-E48E9C287715}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Clary Capt Deryk L:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Power draw when heating in kilowatts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{CA22DA69-A337-4697-92E5-7140B25277EF}">
       <text>
         <r>
           <rPr>
@@ -160,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{2941FCA1-3989-4B87-A58C-A2FC5F222FF8}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{2941FCA1-3989-4B87-A58C-A2FC5F222FF8}">
       <text>
         <r>
           <rPr>
@@ -184,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{777B2B46-B229-402A-817B-98DB020B0070}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{777B2B46-B229-402A-817B-98DB020B0070}">
       <text>
         <r>
           <rPr>
@@ -208,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{497D20C6-4D05-463C-A46C-20AA7191D1C0}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{497D20C6-4D05-463C-A46C-20AA7191D1C0}">
       <text>
         <r>
           <rPr>
@@ -233,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{8CCC2C55-8BF5-4015-B126-BD278BA5DAA1}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{8CCC2C55-8BF5-4015-B126-BD278BA5DAA1}">
       <text>
         <r>
           <rPr>
@@ -258,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{83EBB1B7-07E1-47A4-9C08-CE3DC04175EA}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{83EBB1B7-07E1-47A4-9C08-CE3DC04175EA}">
       <text>
         <r>
           <rPr>
@@ -282,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{05336B23-4DF5-4899-8869-5570723A3FD4}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{05336B23-4DF5-4899-8869-5570723A3FD4}">
       <text>
         <r>
           <rPr>
@@ -306,7 +332,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{FC3D57EC-E239-4FB0-BF44-4EBEB7EC975D}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{FC3D57EC-E239-4FB0-BF44-4EBEB7EC975D}">
       <text>
         <r>
           <rPr>
@@ -359,7 +385,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Unit (ECU)</t>
   </si>
@@ -407,6 +433,9 @@
   </si>
   <si>
     <t>Cooling Load (KW)</t>
+  </si>
+  <si>
+    <t>Heating Load (KW)</t>
   </si>
 </sst>
 </file>
@@ -1324,10 +1353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EEEBF1-4309-4F37-B65A-956648DAA7CF}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,14 +1365,15 @@
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1357,157 +1387,169 @@
         <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2">
-        <v>60000</v>
+        <v>54200</v>
       </c>
       <c r="C2" s="2">
-        <v>37000</v>
+        <v>37100</v>
       </c>
       <c r="D2" s="2">
-        <v>12.9</v>
+        <v>12.231999999999999</v>
       </c>
       <c r="E2" s="2">
+        <v>12.646000000000001</v>
+      </c>
+      <c r="F2" s="2">
         <v>20251</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>560</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>48.4</v>
       </c>
-      <c r="H2" s="2" t="b">
+      <c r="I2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="I2" s="3">
-        <f>E2/B2</f>
-        <v>0.33751666666666669</v>
-      </c>
       <c r="J2" s="3">
+        <f>F2/B2</f>
+        <v>0.37363468634686348</v>
+      </c>
+      <c r="K2" s="3">
         <f>D2/B2</f>
-        <v>2.1499999999999999E-4</v>
-      </c>
-      <c r="K2" s="3">
+        <v>2.2568265682656826E-4</v>
+      </c>
+      <c r="L2" s="3">
+        <f>H2/B2</f>
+        <v>8.9298892988929886E-4</v>
+      </c>
+      <c r="M2" s="4">
         <f>G2/B2</f>
-        <v>8.0666666666666669E-4</v>
-      </c>
-      <c r="L2" s="4">
-        <f>F2/B2</f>
-        <v>9.3333333333333341E-3</v>
+        <v>1.0332103321033211E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>36000</v>
+        <v>34100</v>
       </c>
       <c r="C3" s="2">
         <v>31000</v>
       </c>
       <c r="D3" s="2">
-        <v>7.7</v>
+        <v>7.0380000000000003</v>
       </c>
       <c r="E3" s="2">
+        <v>10.371</v>
+      </c>
+      <c r="F3" s="2">
         <v>15092</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>472</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>43.3</v>
       </c>
-      <c r="H3" s="2" t="b">
+      <c r="I3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="3">
-        <f>E3/B3</f>
-        <v>0.41922222222222222</v>
-      </c>
       <c r="J3" s="3">
+        <f>F3/B3</f>
+        <v>0.44258064516129031</v>
+      </c>
+      <c r="K3" s="3">
         <f>D3/B3</f>
-        <v>2.138888888888889E-4</v>
-      </c>
-      <c r="K3" s="3">
+        <v>2.0639296187683286E-4</v>
+      </c>
+      <c r="L3" s="3">
+        <f>H3/B3</f>
+        <v>1.2697947214076245E-3</v>
+      </c>
+      <c r="M3" s="4">
         <f>G3/B3</f>
-        <v>1.2027777777777777E-3</v>
-      </c>
-      <c r="L3" s="4">
-        <f>F3/B3</f>
-        <v>1.3111111111111112E-2</v>
+        <v>1.3841642228739003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>18000</v>
+        <v>18500</v>
       </c>
       <c r="C4" s="2">
-        <v>14700</v>
+        <v>14300</v>
       </c>
       <c r="D4" s="2">
-        <v>5.0999999999999996</v>
+        <v>4.9050000000000002</v>
       </c>
       <c r="E4" s="2">
+        <v>4.9560000000000004</v>
+      </c>
+      <c r="F4" s="2">
         <v>10020.66</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>230</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>9.6999999999999993</v>
       </c>
-      <c r="H4" s="2" t="b">
+      <c r="I4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="I4" s="3">
-        <f>E4/B4</f>
-        <v>0.55670333333333333</v>
-      </c>
       <c r="J4" s="3">
+        <f>F4/B4</f>
+        <v>0.54165729729729728</v>
+      </c>
+      <c r="K4" s="3">
         <f>D4/B4</f>
-        <v>2.833333333333333E-4</v>
-      </c>
-      <c r="K4" s="3">
+        <v>2.6513513513513513E-4</v>
+      </c>
+      <c r="L4" s="3">
+        <f>H4/B4</f>
+        <v>5.2432432432432429E-4</v>
+      </c>
+      <c r="M4" s="4">
         <f>G4/B4</f>
-        <v>5.3888888888888888E-4</v>
-      </c>
-      <c r="L4" s="4">
-        <f>F4/B4</f>
-        <v>1.2777777777777779E-2</v>
+        <v>1.2432432432432432E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1521,31 +1563,34 @@
         <v>21.1</v>
       </c>
       <c r="E5" s="2">
+        <v>11.7</v>
+      </c>
+      <c r="F5" s="2">
         <v>22000</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>540</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>30.18</v>
       </c>
-      <c r="H5" s="2" t="b">
+      <c r="I5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="3">
-        <f>E5/B5</f>
+      <c r="J5" s="3">
+        <f>F5/B5</f>
         <v>0.30555555555555558</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <f>D5/B5</f>
         <v>2.9305555555555557E-4</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
+        <f>H5/B5</f>
+        <v>4.1916666666666665E-4</v>
+      </c>
+      <c r="M5" s="4">
         <f>G5/B5</f>
-        <v>4.1916666666666665E-4</v>
-      </c>
-      <c r="L5" s="4">
-        <f>F5/B5</f>
         <v>7.4999999999999997E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add heating support, custom generators, and UI improvements (#32)
* Add heating support, custom generators, and UI improvements

Major update to app adding support for:
- added ability to handle heating tents in cold weather environments
- custom generator file uploads
- E2O logo display in app
- improved UI dialogs.

The MILP formulation and ECU input files were updated to support new data for heating and cooling.
Requirements updated to include gitpython for update date display.
Various bug fixes, refactoring, and enhancements to plotting, data validation, and user feedback.
</commit_message>
<xml_diff>
--- a/Inputs/ECUSpecs.xlsx
+++ b/Inputs/ECUSpecs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmc-my.sharepoint-mil.us/personal/deryk_l_clary_mil_usmc_mil/Documents/Documents/VS Code/1. Air Conditioners/Inputs/XLS Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmc-my.sharepoint-mil.us/personal/deryk_l_clary_mil_usmc_mil/Documents/Documents/VS Code/1. Air Conditioners/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{119B4761-BC1C-411D-80A4-A6DC2720C6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2586C56C-4A96-49B5-9E04-EAD45C933CBC}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{119B4761-BC1C-411D-80A4-A6DC2720C6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19562F0D-D24C-4BE5-B6F1-537A969544A0}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="90" windowWidth="29040" windowHeight="15510" xr2:uid="{60A86E40-7E2F-4C45-AF44-FF6C3ADE04BA}"/>
+    <workbookView xWindow="30045" yWindow="1845" windowWidth="21600" windowHeight="11070" xr2:uid="{60A86E40-7E2F-4C45-AF44-FF6C3ADE04BA}"/>
   </bookViews>
   <sheets>
     <sheet name="ECUSpecs" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-The maximum BTU/hr capacity</t>
+The maximum BTU/hr capacity
+Using "@ 125 degrees" metrics.</t>
         </r>
       </text>
     </comment>
@@ -131,11 +132,36 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-The maximum amount of electrical load produced by the unit.</t>
+The maximum amount of electrical load produced by the unit.
+Using "@ 125 degrees" metrics.</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{CA22DA69-A337-4697-92E5-7140B25277EF}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{7753F88A-6B92-4534-9A04-E48E9C287715}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Clary Capt Deryk L:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Power draw when heating in kilowatts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{CA22DA69-A337-4697-92E5-7140B25277EF}">
       <text>
         <r>
           <rPr>
@@ -160,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{2941FCA1-3989-4B87-A58C-A2FC5F222FF8}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{2941FCA1-3989-4B87-A58C-A2FC5F222FF8}">
       <text>
         <r>
           <rPr>
@@ -184,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{777B2B46-B229-402A-817B-98DB020B0070}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{777B2B46-B229-402A-817B-98DB020B0070}">
       <text>
         <r>
           <rPr>
@@ -208,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{497D20C6-4D05-463C-A46C-20AA7191D1C0}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{497D20C6-4D05-463C-A46C-20AA7191D1C0}">
       <text>
         <r>
           <rPr>
@@ -233,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{8CCC2C55-8BF5-4015-B126-BD278BA5DAA1}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{8CCC2C55-8BF5-4015-B126-BD278BA5DAA1}">
       <text>
         <r>
           <rPr>
@@ -258,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{83EBB1B7-07E1-47A4-9C08-CE3DC04175EA}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{83EBB1B7-07E1-47A4-9C08-CE3DC04175EA}">
       <text>
         <r>
           <rPr>
@@ -282,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{05336B23-4DF5-4899-8869-5570723A3FD4}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{05336B23-4DF5-4899-8869-5570723A3FD4}">
       <text>
         <r>
           <rPr>
@@ -306,7 +332,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{FC3D57EC-E239-4FB0-BF44-4EBEB7EC975D}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{FC3D57EC-E239-4FB0-BF44-4EBEB7EC975D}">
       <text>
         <r>
           <rPr>
@@ -359,7 +385,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Unit (ECU)</t>
   </si>
@@ -407,6 +433,9 @@
   </si>
   <si>
     <t>Cooling Load (KW)</t>
+  </si>
+  <si>
+    <t>Heating Load (KW)</t>
   </si>
 </sst>
 </file>
@@ -1324,10 +1353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EEEBF1-4309-4F37-B65A-956648DAA7CF}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,14 +1365,15 @@
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1357,157 +1387,169 @@
         <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2">
-        <v>60000</v>
+        <v>54200</v>
       </c>
       <c r="C2" s="2">
-        <v>37000</v>
+        <v>37100</v>
       </c>
       <c r="D2" s="2">
-        <v>12.9</v>
+        <v>12.231999999999999</v>
       </c>
       <c r="E2" s="2">
+        <v>12.646000000000001</v>
+      </c>
+      <c r="F2" s="2">
         <v>20251</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>560</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>48.4</v>
       </c>
-      <c r="H2" s="2" t="b">
+      <c r="I2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="I2" s="3">
-        <f>E2/B2</f>
-        <v>0.33751666666666669</v>
-      </c>
       <c r="J2" s="3">
+        <f>F2/B2</f>
+        <v>0.37363468634686348</v>
+      </c>
+      <c r="K2" s="3">
         <f>D2/B2</f>
-        <v>2.1499999999999999E-4</v>
-      </c>
-      <c r="K2" s="3">
+        <v>2.2568265682656826E-4</v>
+      </c>
+      <c r="L2" s="3">
+        <f>H2/B2</f>
+        <v>8.9298892988929886E-4</v>
+      </c>
+      <c r="M2" s="4">
         <f>G2/B2</f>
-        <v>8.0666666666666669E-4</v>
-      </c>
-      <c r="L2" s="4">
-        <f>F2/B2</f>
-        <v>9.3333333333333341E-3</v>
+        <v>1.0332103321033211E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>36000</v>
+        <v>34100</v>
       </c>
       <c r="C3" s="2">
         <v>31000</v>
       </c>
       <c r="D3" s="2">
-        <v>7.7</v>
+        <v>7.0380000000000003</v>
       </c>
       <c r="E3" s="2">
+        <v>10.371</v>
+      </c>
+      <c r="F3" s="2">
         <v>15092</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>472</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>43.3</v>
       </c>
-      <c r="H3" s="2" t="b">
+      <c r="I3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="3">
-        <f>E3/B3</f>
-        <v>0.41922222222222222</v>
-      </c>
       <c r="J3" s="3">
+        <f>F3/B3</f>
+        <v>0.44258064516129031</v>
+      </c>
+      <c r="K3" s="3">
         <f>D3/B3</f>
-        <v>2.138888888888889E-4</v>
-      </c>
-      <c r="K3" s="3">
+        <v>2.0639296187683286E-4</v>
+      </c>
+      <c r="L3" s="3">
+        <f>H3/B3</f>
+        <v>1.2697947214076245E-3</v>
+      </c>
+      <c r="M3" s="4">
         <f>G3/B3</f>
-        <v>1.2027777777777777E-3</v>
-      </c>
-      <c r="L3" s="4">
-        <f>F3/B3</f>
-        <v>1.3111111111111112E-2</v>
+        <v>1.3841642228739003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>18000</v>
+        <v>18500</v>
       </c>
       <c r="C4" s="2">
-        <v>14700</v>
+        <v>14300</v>
       </c>
       <c r="D4" s="2">
-        <v>5.0999999999999996</v>
+        <v>4.9050000000000002</v>
       </c>
       <c r="E4" s="2">
+        <v>4.9560000000000004</v>
+      </c>
+      <c r="F4" s="2">
         <v>10020.66</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>230</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>9.6999999999999993</v>
       </c>
-      <c r="H4" s="2" t="b">
+      <c r="I4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="I4" s="3">
-        <f>E4/B4</f>
-        <v>0.55670333333333333</v>
-      </c>
       <c r="J4" s="3">
+        <f>F4/B4</f>
+        <v>0.54165729729729728</v>
+      </c>
+      <c r="K4" s="3">
         <f>D4/B4</f>
-        <v>2.833333333333333E-4</v>
-      </c>
-      <c r="K4" s="3">
+        <v>2.6513513513513513E-4</v>
+      </c>
+      <c r="L4" s="3">
+        <f>H4/B4</f>
+        <v>5.2432432432432429E-4</v>
+      </c>
+      <c r="M4" s="4">
         <f>G4/B4</f>
-        <v>5.3888888888888888E-4</v>
-      </c>
-      <c r="L4" s="4">
-        <f>F4/B4</f>
-        <v>1.2777777777777779E-2</v>
+        <v>1.2432432432432432E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1521,31 +1563,34 @@
         <v>21.1</v>
       </c>
       <c r="E5" s="2">
+        <v>11.7</v>
+      </c>
+      <c r="F5" s="2">
         <v>22000</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>540</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>30.18</v>
       </c>
-      <c r="H5" s="2" t="b">
+      <c r="I5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="3">
-        <f>E5/B5</f>
+      <c r="J5" s="3">
+        <f>F5/B5</f>
         <v>0.30555555555555558</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <f>D5/B5</f>
         <v>2.9305555555555557E-4</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
+        <f>H5/B5</f>
+        <v>4.1916666666666665E-4</v>
+      </c>
+      <c r="M5" s="4">
         <f>G5/B5</f>
-        <v>4.1916666666666665E-4</v>
-      </c>
-      <c r="L5" s="4">
-        <f>F5/B5</f>
         <v>7.4999999999999997E-3</v>
       </c>
     </row>

</xml_diff>